<commit_message>
Instructions for the Migration of 'Bildgattungen'
</commit_message>
<xml_diff>
--- a/Excel_Mapping/Genre_List_To_XML.xlsx
+++ b/Excel_Mapping/Genre_List_To_XML.xlsx
@@ -24,23 +24,40 @@
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="135.69pt"/>
+    </style:style>
+    <style:style style:name="co2" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="155.71pt"/>
+    </style:style>
+    <style:style style:name="co3" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="64.01pt"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
-      <style:table-row-properties style:row-height="132.29pt" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="13.86pt" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro2" style:family="table-row">
+      <style:table-row-properties style:row-height="55.5pt" fo:break-before="auto" style:use-optimal-row-height="false"/>
+    </style:style>
+    <style:style style:name="ro3" style:family="table-row">
       <style:table-row-properties style:row-height="12.81pt" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
+    </style:style>
+    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#dddddd"/>
+    </style:style>
+    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#ffff00"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="Sheet1" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:number-columns-repeated="6" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co3" table:number-columns-repeated="4" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>&lt;item idno="</text:p>
@@ -54,26 +71,16 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;item idno="persons" enabled="1" default="0" value="0"&gt;</text:p>
-            <text:p>          &lt;labels&gt;</text:p>
-            <text:p>            &lt;label locale="de_CH" preferred="1"&gt;</text:p>
-            <text:p>              &lt;name_singular&gt;Person&lt;/name_singular&gt;</text:p>
-            <text:p>              &lt;name_plural&gt;Personen&lt;/name_plural&gt;</text:p>
-            <text:p>            &lt;/label&gt;</text:p>
-            <text:p>            &lt;label locale="en_US" preferred="1"&gt;</text:p>
-            <text:p>              &lt;name_singular&gt;Person&lt;/name_singular&gt;</text:p>
-            <text:p>              &lt;name_plural&gt;Persons&lt;/name_plural&gt;</text:p>
-            <text:p>            &lt;/label&gt;</text:p>
-            <text:p>          &lt;/labels&gt;</text:p>
-            <text:p>        &lt;/item&gt;</text:p>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:s/>
+            </text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell table:number-columns-repeated="6"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Personen</text:p>
           </table:table-cell>
@@ -85,7 +92,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Reportage</text:p>
           </table:table-cell>
@@ -97,7 +104,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Presse</text:p>
           </table:table-cell>
@@ -109,11 +116,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Portraet</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A6])" office:value-type="string" office:string-value="portraet" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A6])" office:value-type="string" office:string-value="portraet" calcext:value-type="string">
             <text:p>portraet</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B6]&amp;[.B$1]&amp;[.A6]&amp;[.C$1]&amp;[.A6]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;portraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Portraet&lt;/name_singular&gt;&lt;name_plural&gt;Portraet&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -121,7 +128,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Ortsbild</text:p>
           </table:table-cell>
@@ -133,7 +140,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Architektur</text:p>
           </table:table-cell>
@@ -145,7 +152,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Landschaft</text:p>
           </table:table-cell>
@@ -157,7 +164,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Natur</text:p>
           </table:table-cell>
@@ -169,7 +176,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Bergfotografie</text:p>
           </table:table-cell>
@@ -181,7 +188,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Flugaufnahme</text:p>
           </table:table-cell>
@@ -193,7 +200,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Gewerbe</text:p>
           </table:table-cell>
@@ -205,7 +212,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Industrie</text:p>
           </table:table-cell>
@@ -217,7 +224,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Tourismus</text:p>
           </table:table-cell>
@@ -229,7 +236,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Landwirtschaft</text:p>
           </table:table-cell>
@@ -241,7 +248,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Tiere</text:p>
           </table:table-cell>
@@ -253,7 +260,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Sachaufnahme</text:p>
           </table:table-cell>
@@ -265,7 +272,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Reproduktion</text:p>
           </table:table-cell>
@@ -277,7 +284,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Werbung</text:p>
           </table:table-cell>
@@ -289,7 +296,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Mode</text:p>
           </table:table-cell>
@@ -301,11 +308,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Firmenportraet</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A22])" office:value-type="string" office:string-value="firmenportraet" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A22])" office:value-type="string" office:string-value="firmenportraet" calcext:value-type="string">
             <text:p>firmenportraet</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B22]&amp;[.B$1]&amp;[.A22]&amp;[.C$1]&amp;[.A22]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;firmenportraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Firmenportraet&lt;/name_singular&gt;&lt;name_plural&gt;Firmenportraet&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -313,7 +320,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Sport</text:p>
           </table:table-cell>
@@ -325,11 +332,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>Unfall / Katastrophe</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>unfall</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B24]&amp;[.B$1]&amp;[.A24]&amp;[.C$1]&amp;[.A24]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;unfall&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Unfall / Katastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Unfall / Katastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -337,7 +344,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Verkehr</text:p>
           </table:table-cell>
@@ -349,11 +356,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Militaer</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A26])" office:value-type="string" office:string-value="militaer" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A26])" office:value-type="string" office:string-value="militaer" calcext:value-type="string">
             <text:p>militaer</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B26]&amp;[.B$1]&amp;[.A26]&amp;[.C$1]&amp;[.A26]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;militaer&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militaer&lt;/name_singular&gt;&lt;name_plural&gt;Militaer&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -361,7 +368,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Ethnologie</text:p>
           </table:table-cell>
@@ -373,11 +380,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Archaeologie</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A28])" office:value-type="string" office:string-value="archaeologie" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A28])" office:value-type="string" office:string-value="archaeologie" calcext:value-type="string">
             <text:p>archaeologie</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B28]&amp;[.B$1]&amp;[.A28]&amp;[.C$1]&amp;[.A28]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;archaeologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archaeologie&lt;/name_singular&gt;&lt;name_plural&gt;Archaeologie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -385,7 +392,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Medizin</text:p>
           </table:table-cell>
@@ -397,7 +404,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Kriminologie</text:p>
           </table:table-cell>
@@ -409,7 +416,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Musik</text:p>
           </table:table-cell>
@@ -421,7 +428,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Theater</text:p>
           </table:table-cell>
@@ -433,7 +440,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Kunst</text:p>
           </table:table-cell>
@@ -445,7 +452,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Literatur</text:p>
           </table:table-cell>
@@ -457,7 +464,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Piktorialismus</text:p>
           </table:table-cell>
@@ -469,11 +476,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>Kunst mit Fotografie</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>kunst_fotografie</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B36]&amp;[.B$1]&amp;[.A36]&amp;[.C$1]&amp;[.A36]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;kunst_fotografie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kunst mit Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;Kunst mit Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -481,7 +488,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Alltag</text:p>
           </table:table-cell>
@@ -493,7 +500,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Akt</text:p>
           </table:table-cell>
@@ -505,7 +512,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Film</text:p>
           </table:table-cell>
@@ -517,7 +524,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Dokumentation</text:p>
           </table:table-cell>
@@ -529,7 +536,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Multivision</text:p>
           </table:table-cell>
@@ -541,11 +548,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>private Fotografie</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>private</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B42]&amp;[.B$1]&amp;[.A42]&amp;[.C$1]&amp;[.A42]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;private&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;private Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;private Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -553,11 +560,11 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>wissenschaftliche Fotografie</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>wissenschaft</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[.A$1]&amp;[.B43]&amp;[.B$1]&amp;[.A43]&amp;[.C$1]&amp;[.A43]&amp;[.D$1]" office:value-type="string" office:string-value="&lt;item idno=&quot;wissenschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;wissenschaftliche Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;wissenschaftliche Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
@@ -565,7 +572,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Reise</text:p>
           </table:table-cell>
@@ -588,11 +595,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2018-09-27T13:59:53.251000000</meta:creation-date>
-    <dc:date>2018-09-27T15:02:45.600000000</dc:date>
-    <meta:editing-duration>PT25M2S</meta:editing-duration>
-    <meta:editing-cycles>4</meta:editing-cycles>
+    <dc:date>2018-09-28T12:36:36.408000000</dc:date>
+    <meta:editing-duration>PT26M44S</meta:editing-duration>
+    <meta:editing-cycles>7</meta:editing-cycles>
     <meta:generator>LibreOffice/5.3.3.2$Windows_X86_64 LibreOffice_project/3d9a8b4b4e538a85e0782bd6c2d430bafe583448</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="131" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="132" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -603,15 +610,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">13546</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">24084</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">19311</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">21411</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">2</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">21</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -620,7 +627,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">12</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -674,8 +681,8 @@
       <config:config-item config:name="IsRasterAxisSynchronized" config:type="boolean">true</config:config-item>
       <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterName" config:type="string">XRX9C934E5563E0</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">pnb+/1hSWDlDOTM0RTU1NjNFMAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWGVyb3ggV29ya0NlbnRyZSA3ODMwIFY0IFBDTDYAAAAWAAEAwnUAAAAAAAAIAFZUAAAkbQAAM1ROVwAAAAAKAFgAUgBYADkAQwA5ADMANABFADUANQA2ADMARQAwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABBAMG3ADcdEO/AQIBAAEA6gpvCGQAAQAPAFgCAgACAFgCAwABAEwAZQB0AHQAZQByAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAQAAAAIAAAAJAQAA/////0dJUzQAAAAAAAAAAAAAAABESU5VIgAAAlwEgHAasavnAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABAAAAAAAAAAAAAfAAAAAAAAAAEAAAAXABQAAQAAAAAAAAABAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAIAAFNNVEoAAAAAEADwAXsAMwAzAGQAMwAyADIAZgBjAC0ANQA4ADQAYgAtADQAMwBmADQALQA5ADMAZAAzAC0AZgA2AGEAZgAwADIAMgA4ADUAOAA0AGQAfQAAAElucHV0QmluAEZPUk1TT1VSQ0UAUkVTRExMAFVuaXJlc0RMTABMb2NhbGUARW5nbGlzaF9Vbml0ZWRfU3RhdGVzAFBhcGVyU2l6ZQBMRVRURVIAT3JpZW50YXRpb24AUE9SVFJBSVQAQ29sb3JNb2RlAENvbG9yAFJlc29sdXRpb24AUmVzXzYwMHg2MDAARHVwbGV4AFZFUlRJQ0FMAEpvYk5VcEFsbERvY3VtZW50c0NvbnRpZ3VvdXNseQAxAE1lZGlhVHlwZQBzdGF0aW9uZXJ5LWxldHRlcmhlYWQATWVkaWFDb2xvcgB3aGl0ZQBDb2xsYXRlAE9OAFN0YXBsaW5nAE5vbmUAU2VjdXJlUHJpbnQAT0ZGAEpvYlBhc3Njb2RlAE9GRgBKb2JJZGVudGlmaWNhdGlvbgBKb2JJZEJhbm5lck9uAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAACAcAAAVjRETQEAAAAAAAAAqkxz8xwAAAAAAQAAAwAAAPwi0zNLWPRDk9P2rwIoWE3kAAAATAAAAAMAAABAAAAAAAAAAAAAAAADAAAAQB8AACoAAABAAAAAAwAAAABQAABiAAAAgB8AAEoAbwBiAFMAaQBtAHAAbABlAFMAZQBjAHUAcgBlAFAAcgBpAG4AdAAAAEoAbwBiAFgAZQByAG8AeABDAG8AbQBwAGwAZQB0AGUARABvAGMAUwBlAHQAdABpAG4AZwBzAAAASgBvAGIAWABlAHIAbwB4AFAAdQBiAGwAaQBjAEQAbwBjAFMAZQB0AHQAaQBuAGcAcwAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAASAENPTVBBVF9EVVBMRVhfTU9ERRQARHVwbGV4TW9kZTo6TG9uZ0VkZ2U=</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
       <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
@@ -683,6 +690,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
       <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
     </config:config-item-set>
   </office:settings>
 </office:document-settings>
@@ -812,9 +820,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2018-09-27">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2018-09-28">00/00/0000</text:date>
             , 
-            <text:time>00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="11:23:58.721000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
Genre List translation fix
</commit_message>
<xml_diff>
--- a/Excel_Mapping/Genre_List_To_XML.xlsx
+++ b/Excel_Mapping/Genre_List_To_XML.xlsx
@@ -53,6 +53,13 @@
     <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
     </style:style>
+    <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#eeeeee"/>
+      <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce8" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#eeeeee"/>
+    </style:style>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
@@ -90,622 +97,622 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>idno</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Total</text:p>
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>Export</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Personen</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A3])" office:value-type="string" office:string-value="personen" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>personen</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A3]&amp;[Snippets.$C$17]&amp;[Translations.A3]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B3]&amp;[Snippets.$C$18]&amp;[Translations.B3]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C3]&amp;[Snippets.$C$19]&amp;[Translations.C3]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D3]&amp;[Snippets.$C$20]&amp;[Translations.D3]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E3]&amp;[Snippets.$C$21]&amp;[Translations.E3]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B3]&amp;[Snippets.$C$18]&amp;[Translations.B3]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C3]&amp;[Snippets.$C$19]&amp;[Translations.C3]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D3]&amp;[Snippets.$C$20]&amp;[Translations.D3]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E3]&amp;[Snippets.$C$21]&amp;[Translations.E3]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B3]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;personen&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="personen" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H3]&amp;[Snippets.B$16]&amp;[.C3]&amp;[.D3]&amp;[.E3]&amp;[.F3]&amp;[.G3]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;personen&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="personen" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H3]&amp;[Snippets.B$16]&amp;[.C3]&amp;[.D3]&amp;[.E3]&amp;[.F3]&amp;[.G3]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;personen&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="personen" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Personne&lt;/name_singular&gt;&lt;name_plural&gt;Personne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Persona&lt;/name_singular&gt;&lt;name_plural&gt;Persona&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Persunas&lt;/name_singular&gt;&lt;name_plural&gt;Persunas&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;People&lt;/name_singular&gt;&lt;name_plural&gt;People&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Reportage</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A4])" office:value-type="string" office:string-value="reportage" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>reportage</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A4]&amp;[Snippets.$C$17]&amp;[Translations.A4]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B4]&amp;[Snippets.$C$18]&amp;[Translations.B4]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C4]&amp;[Snippets.$C$19]&amp;[Translations.C4]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D4]&amp;[Snippets.$C$20]&amp;[Translations.D4]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E4]&amp;[Snippets.$C$21]&amp;[Translations.E4]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B4]&amp;[Snippets.$C$18]&amp;[Translations.B4]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C4]&amp;[Snippets.$C$19]&amp;[Translations.C4]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D4]&amp;[Snippets.$C$20]&amp;[Translations.D4]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E4]&amp;[Snippets.$C$21]&amp;[Translations.E4]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B4]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;reportage&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="reportage" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H4]&amp;[Snippets.B$16]&amp;[.C4]&amp;[.D4]&amp;[.E4]&amp;[.F4]&amp;[.G4]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;reportage&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="reportage" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H4]&amp;[Snippets.B$16]&amp;[.C4]&amp;[.D4]&amp;[.E4]&amp;[.F4]&amp;[.G4]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;reportage&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="reportage" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Reportascha&lt;/name_singular&gt;&lt;name_plural&gt;Reportascha&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Reportage&lt;/name_singular&gt;&lt;name_plural&gt;Reportage&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Presse</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A5])" office:value-type="string" office:string-value="presse" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>presse</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A5]&amp;[Snippets.$C$17]&amp;[Translations.A5]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Presse&lt;/name_singular&gt;&lt;name_plural&gt;Presse&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Presse&lt;/name_singular&gt;&lt;name_plural&gt;Presse&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B5]&amp;[Snippets.$C$18]&amp;[Translations.B5]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C5]&amp;[Snippets.$C$19]&amp;[Translations.C5]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D5]&amp;[Snippets.$C$20]&amp;[Translations.D5]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E5]&amp;[Snippets.$C$21]&amp;[Translations.E5]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B5]&amp;[Snippets.$C$18]&amp;[Translations.B5]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C5]&amp;[Snippets.$C$19]&amp;[Translations.C5]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D5]&amp;[Snippets.$C$20]&amp;[Translations.D5]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E5]&amp;[Snippets.$C$21]&amp;[Translations.E5]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B5]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;presse&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="presse" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H5]&amp;[Snippets.B$16]&amp;[.C5]&amp;[.D5]&amp;[.E5]&amp;[.F5]&amp;[.G5]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;presse&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Presse&lt;/name_singular&gt;&lt;name_plural&gt;Presse&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="presse" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Presse&lt;/name_singular&gt;&lt;name_plural&gt;Presse&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H5]&amp;[Snippets.B$16]&amp;[.C5]&amp;[.D5]&amp;[.E5]&amp;[.F5]&amp;[.G5]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;presse&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Presse&lt;/name_singular&gt;&lt;name_plural&gt;Presse&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="presse" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Presse&lt;/name_singular&gt;&lt;name_plural&gt;Presse&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photojournalisme&lt;/name_singular&gt;&lt;name_plural&gt;Photojournalisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotogiornalismo&lt;/name_singular&gt;&lt;name_plural&gt;Fotogiornalismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Pressa&lt;/name_singular&gt;&lt;name_plural&gt;Pressa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Press&lt;/name_singular&gt;&lt;name_plural&gt;Press&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
-            <text:p>Portraet</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A6])" office:value-type="string" office:string-value="portraet" calcext:value-type="string">
+            <text:p>Porträt</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>portraet</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A6]&amp;[Snippets.$C$17]&amp;[Translations.A6]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Porträt&lt;/name_singular&gt;&lt;name_plural&gt;Porträt&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Porträt&lt;/name_singular&gt;&lt;name_plural&gt;Porträt&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B6]&amp;[Snippets.$C$18]&amp;[Translations.B6]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C6]&amp;[Snippets.$C$19]&amp;[Translations.C6]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D6]&amp;[Snippets.$C$20]&amp;[Translations.D6]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E6]&amp;[Snippets.$C$21]&amp;[Translations.E6]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B6]&amp;[Snippets.$C$18]&amp;[Translations.B6]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C6]&amp;[Snippets.$C$19]&amp;[Translations.C6]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D6]&amp;[Snippets.$C$20]&amp;[Translations.D6]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E6]&amp;[Snippets.$C$21]&amp;[Translations.E6]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B6]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;portraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="portraet" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H6]&amp;[Snippets.B$16]&amp;[.C6]&amp;[.D6]&amp;[.E6]&amp;[.F6]&amp;[.G6]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;portraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Porträt&lt;/name_singular&gt;&lt;name_plural&gt;Porträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="portraet" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Porträt&lt;/name_singular&gt;&lt;name_plural&gt;Porträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H6]&amp;[Snippets.B$16]&amp;[.C6]&amp;[.D6]&amp;[.E6]&amp;[.F6]&amp;[.G6]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;portraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Porträt&lt;/name_singular&gt;&lt;name_plural&gt;Porträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="portraet" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Porträt&lt;/name_singular&gt;&lt;name_plural&gt;Porträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Ritratto&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Purtret&lt;/name_singular&gt;&lt;name_plural&gt;Purtret&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Portrait&lt;/name_singular&gt;&lt;name_plural&gt;Portrait&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Ortsbild</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A7])" office:value-type="string" office:string-value="ortsbild" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ortsbild</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A7]&amp;[Snippets.$C$17]&amp;[Translations.A7]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ortsbild&lt;/name_singular&gt;&lt;name_plural&gt;Ortsbild&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Ortsbild&lt;/name_singular&gt;&lt;name_plural&gt;Ortsbild&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B7]&amp;[Snippets.$C$18]&amp;[Translations.B7]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C7]&amp;[Snippets.$C$19]&amp;[Translations.C7]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D7]&amp;[Snippets.$C$20]&amp;[Translations.D7]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E7]&amp;[Snippets.$C$21]&amp;[Translations.E7]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B7]&amp;[Snippets.$C$18]&amp;[Translations.B7]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C7]&amp;[Snippets.$C$19]&amp;[Translations.C7]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D7]&amp;[Snippets.$C$20]&amp;[Translations.D7]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E7]&amp;[Snippets.$C$21]&amp;[Translations.E7]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B7]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;ortsbild&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="ortsbild" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H7]&amp;[Snippets.B$16]&amp;[.C7]&amp;[.D7]&amp;[.E7]&amp;[.F7]&amp;[.G7]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;ortsbild&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ortsbild&lt;/name_singular&gt;&lt;name_plural&gt;Ortsbild&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="ortsbild" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Ortsbild&lt;/name_singular&gt;&lt;name_plural&gt;Ortsbild&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H7]&amp;[Snippets.B$16]&amp;[.C7]&amp;[.D7]&amp;[.E7]&amp;[.F7]&amp;[.G7]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;ortsbild&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ortsbild&lt;/name_singular&gt;&lt;name_plural&gt;Ortsbild&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="ortsbild" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Ortsbild&lt;/name_singular&gt;&lt;name_plural&gt;Ortsbild&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Paysage urbain&lt;/name_singular&gt;&lt;name_plural&gt;Paysage urbain&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Paesaggio urbano&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio urbano&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Maletg dal vitg&lt;/name_singular&gt;&lt;name_plural&gt;Maletg dal vitg&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Townscape&lt;/name_singular&gt;&lt;name_plural&gt;Townscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Architektur</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A8])" office:value-type="string" office:string-value="architektur" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>architektur</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A8]&amp;[Snippets.$C$17]&amp;[Translations.A8]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architektur&lt;/name_singular&gt;&lt;name_plural&gt;Architektur&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Architektur&lt;/name_singular&gt;&lt;name_plural&gt;Architektur&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B8]&amp;[Snippets.$C$18]&amp;[Translations.B8]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C8]&amp;[Snippets.$C$19]&amp;[Translations.C8]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D8]&amp;[Snippets.$C$20]&amp;[Translations.D8]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E8]&amp;[Snippets.$C$21]&amp;[Translations.E8]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B8]&amp;[Snippets.$C$18]&amp;[Translations.B8]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C8]&amp;[Snippets.$C$19]&amp;[Translations.C8]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D8]&amp;[Snippets.$C$20]&amp;[Translations.D8]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E8]&amp;[Snippets.$C$21]&amp;[Translations.E8]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B8]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;architektur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="architektur" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H8]&amp;[Snippets.B$16]&amp;[.C8]&amp;[.D8]&amp;[.E8]&amp;[.F8]&amp;[.G8]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;architektur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architektur&lt;/name_singular&gt;&lt;name_plural&gt;Architektur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="architektur" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Architektur&lt;/name_singular&gt;&lt;name_plural&gt;Architektur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H8]&amp;[Snippets.B$16]&amp;[.C8]&amp;[.D8]&amp;[.E8]&amp;[.F8]&amp;[.G8]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;architektur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architektur&lt;/name_singular&gt;&lt;name_plural&gt;Architektur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="architektur" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Architektur&lt;/name_singular&gt;&lt;name_plural&gt;Architektur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Architettura&lt;/name_singular&gt;&lt;name_plural&gt;Architettura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Architectura&lt;/name_singular&gt;&lt;name_plural&gt;Architectura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Architecture&lt;/name_singular&gt;&lt;name_plural&gt;Architecture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Landschaft</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A9])" office:value-type="string" office:string-value="landschaft" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>landschaft</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A9]&amp;[Snippets.$C$17]&amp;[Translations.A9]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landschaft&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Landschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landschaft&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B9]&amp;[Snippets.$C$18]&amp;[Translations.B9]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C9]&amp;[Snippets.$C$19]&amp;[Translations.C9]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D9]&amp;[Snippets.$C$20]&amp;[Translations.D9]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E9]&amp;[Snippets.$C$21]&amp;[Translations.E9]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B9]&amp;[Snippets.$C$18]&amp;[Translations.B9]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C9]&amp;[Snippets.$C$19]&amp;[Translations.C9]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D9]&amp;[Snippets.$C$20]&amp;[Translations.D9]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E9]&amp;[Snippets.$C$21]&amp;[Translations.E9]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B9]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;landschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="landschaft" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H9]&amp;[Snippets.B$16]&amp;[.C9]&amp;[.D9]&amp;[.E9]&amp;[.F9]&amp;[.G9]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;landschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="landschaft" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Landschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H9]&amp;[Snippets.B$16]&amp;[.C9]&amp;[.D9]&amp;[.E9]&amp;[.F9]&amp;[.G9]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;landschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="landschaft" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Landschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Paysage&lt;/name_singular&gt;&lt;name_plural&gt;Paysage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Paesaggio&lt;/name_singular&gt;&lt;name_plural&gt;Paesaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Cuntrada&lt;/name_singular&gt;&lt;name_plural&gt;Cuntrada&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Landscape&lt;/name_singular&gt;&lt;name_plural&gt;Landscape&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Natur</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A10])" office:value-type="string" office:string-value="natur" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>natur</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A10]&amp;[Snippets.$C$17]&amp;[Translations.A10]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Natur&lt;/name_singular&gt;&lt;name_plural&gt;Natur&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Natur&lt;/name_singular&gt;&lt;name_plural&gt;Natur&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B10]&amp;[Snippets.$C$18]&amp;[Translations.B10]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C10]&amp;[Snippets.$C$19]&amp;[Translations.C10]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D10]&amp;[Snippets.$C$20]&amp;[Translations.D10]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E10]&amp;[Snippets.$C$21]&amp;[Translations.E10]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B10]&amp;[Snippets.$C$18]&amp;[Translations.B10]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C10]&amp;[Snippets.$C$19]&amp;[Translations.C10]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D10]&amp;[Snippets.$C$20]&amp;[Translations.D10]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E10]&amp;[Snippets.$C$21]&amp;[Translations.E10]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B10]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;natur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="natur" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H10]&amp;[Snippets.B$16]&amp;[.C10]&amp;[.D10]&amp;[.E10]&amp;[.F10]&amp;[.G10]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;natur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Natur&lt;/name_singular&gt;&lt;name_plural&gt;Natur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="natur" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Natur&lt;/name_singular&gt;&lt;name_plural&gt;Natur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H10]&amp;[Snippets.B$16]&amp;[.C10]&amp;[.D10]&amp;[.E10]&amp;[.F10]&amp;[.G10]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;natur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Natur&lt;/name_singular&gt;&lt;name_plural&gt;Natur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="natur" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Natur&lt;/name_singular&gt;&lt;name_plural&gt;Natur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Natura&lt;/name_singular&gt;&lt;name_plural&gt;Natura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Natira&lt;/name_singular&gt;&lt;name_plural&gt;Natira&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Nature&lt;/name_singular&gt;&lt;name_plural&gt;Nature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Bergfotografie</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A11])" office:value-type="string" office:string-value="bergfotografie" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>bergfotografie</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A11]&amp;[Snippets.$C$17]&amp;[Translations.A11]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Bergfotografie&lt;/name_singular&gt;&lt;name_plural&gt;Bergfotografie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Bergfotografie&lt;/name_singular&gt;&lt;name_plural&gt;Bergfotografie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B11]&amp;[Snippets.$C$18]&amp;[Translations.B11]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C11]&amp;[Snippets.$C$19]&amp;[Translations.C11]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D11]&amp;[Snippets.$C$20]&amp;[Translations.D11]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E11]&amp;[Snippets.$C$21]&amp;[Translations.E11]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B11]&amp;[Snippets.$C$18]&amp;[Translations.B11]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C11]&amp;[Snippets.$C$19]&amp;[Translations.C11]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D11]&amp;[Snippets.$C$20]&amp;[Translations.D11]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E11]&amp;[Snippets.$C$21]&amp;[Translations.E11]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B11]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;bergfotografie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="bergfotografie" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H11]&amp;[Snippets.B$16]&amp;[.C11]&amp;[.D11]&amp;[.E11]&amp;[.F11]&amp;[.G11]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;bergfotografie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Bergfotografie&lt;/name_singular&gt;&lt;name_plural&gt;Bergfotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="bergfotografie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Bergfotografie&lt;/name_singular&gt;&lt;name_plural&gt;Bergfotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H11]&amp;[Snippets.B$16]&amp;[.C11]&amp;[.D11]&amp;[.E11]&amp;[.F11]&amp;[.G11]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;bergfotografie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Bergfotografie&lt;/name_singular&gt;&lt;name_plural&gt;Bergfotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="bergfotografie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Bergfotografie&lt;/name_singular&gt;&lt;name_plural&gt;Bergfotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie de montagne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie de montagne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia di montagna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia di montagna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia da muntogna&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia da muntogna&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Alpine photography&lt;/name_singular&gt;&lt;name_plural&gt;Alpine photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Flugaufnahme</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A12])" office:value-type="string" office:string-value="flugaufnahme" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>flugaufnahme</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A12]&amp;[Snippets.$C$17]&amp;[Translations.A12]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Flugaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Flugaufnahme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Flugaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Flugaufnahme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B12]&amp;[Snippets.$C$18]&amp;[Translations.B12]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C12]&amp;[Snippets.$C$19]&amp;[Translations.C12]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D12]&amp;[Snippets.$C$20]&amp;[Translations.D12]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E12]&amp;[Snippets.$C$21]&amp;[Translations.E12]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B12]&amp;[Snippets.$C$18]&amp;[Translations.B12]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C12]&amp;[Snippets.$C$19]&amp;[Translations.C12]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D12]&amp;[Snippets.$C$20]&amp;[Translations.D12]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E12]&amp;[Snippets.$C$21]&amp;[Translations.E12]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B12]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;flugaufnahme&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="flugaufnahme" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H12]&amp;[Snippets.B$16]&amp;[.C12]&amp;[.D12]&amp;[.E12]&amp;[.F12]&amp;[.G12]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;flugaufnahme&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Flugaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Flugaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="flugaufnahme" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Flugaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Flugaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H12]&amp;[Snippets.B$16]&amp;[.C12]&amp;[.D12]&amp;[.E12]&amp;[.F12]&amp;[.G12]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;flugaufnahme&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Flugaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Flugaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="flugaufnahme" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Flugaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Flugaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie aérienne&lt;/name_singular&gt;&lt;name_plural&gt;Photographie aérienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia aerea&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia aerea&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia or da l'aria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia or da l'aria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Aerial photography&lt;/name_singular&gt;&lt;name_plural&gt;Aerial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Gewerbe</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A13])" office:value-type="string" office:string-value="gewerbe" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>gewerbe</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A13]&amp;[Snippets.$C$17]&amp;[Translations.A13]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Gewerbe&lt;/name_singular&gt;&lt;name_plural&gt;Gewerbe&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Gewerbe&lt;/name_singular&gt;&lt;name_plural&gt;Gewerbe&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B13]&amp;[Snippets.$C$18]&amp;[Translations.B13]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C13]&amp;[Snippets.$C$19]&amp;[Translations.C13]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D13]&amp;[Snippets.$C$20]&amp;[Translations.D13]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E13]&amp;[Snippets.$C$21]&amp;[Translations.E13]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B13]&amp;[Snippets.$C$18]&amp;[Translations.B13]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C13]&amp;[Snippets.$C$19]&amp;[Translations.C13]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D13]&amp;[Snippets.$C$20]&amp;[Translations.D13]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E13]&amp;[Snippets.$C$21]&amp;[Translations.E13]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B13]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;gewerbe&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="gewerbe" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H13]&amp;[Snippets.B$16]&amp;[.C13]&amp;[.D13]&amp;[.E13]&amp;[.F13]&amp;[.G13]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;gewerbe&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Gewerbe&lt;/name_singular&gt;&lt;name_plural&gt;Gewerbe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="gewerbe" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Gewerbe&lt;/name_singular&gt;&lt;name_plural&gt;Gewerbe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H13]&amp;[Snippets.B$16]&amp;[.C13]&amp;[.D13]&amp;[.E13]&amp;[.F13]&amp;[.G13]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;gewerbe&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Gewerbe&lt;/name_singular&gt;&lt;name_plural&gt;Gewerbe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="gewerbe" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Gewerbe&lt;/name_singular&gt;&lt;name_plural&gt;Gewerbe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Métier&lt;/name_singular&gt;&lt;name_plural&gt;Métier&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Arti e mestieri&lt;/name_singular&gt;&lt;name_plural&gt;Arti e mestieri&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Commerzi&lt;/name_singular&gt;&lt;name_plural&gt;Commerzi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Commercial photography&lt;/name_singular&gt;&lt;name_plural&gt;Commercial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Industrie</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A14])" office:value-type="string" office:string-value="industrie" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>industrie</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A14]&amp;[Snippets.$C$17]&amp;[Translations.A14]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B14]&amp;[Snippets.$C$18]&amp;[Translations.B14]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C14]&amp;[Snippets.$C$19]&amp;[Translations.C14]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D14]&amp;[Snippets.$C$20]&amp;[Translations.D14]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E14]&amp;[Snippets.$C$21]&amp;[Translations.E14]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B14]&amp;[Snippets.$C$18]&amp;[Translations.B14]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C14]&amp;[Snippets.$C$19]&amp;[Translations.C14]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D14]&amp;[Snippets.$C$20]&amp;[Translations.D14]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E14]&amp;[Snippets.$C$21]&amp;[Translations.E14]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B14]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;industrie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="industrie" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H14]&amp;[Snippets.B$16]&amp;[.C14]&amp;[.D14]&amp;[.E14]&amp;[.F14]&amp;[.G14]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;industrie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="industrie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H14]&amp;[Snippets.B$16]&amp;[.C14]&amp;[.D14]&amp;[.E14]&amp;[.F14]&amp;[.G14]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;industrie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="industrie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Industrie&lt;/name_singular&gt;&lt;name_plural&gt;Industrie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Industria&lt;/name_singular&gt;&lt;name_plural&gt;Industria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Industrial photography&lt;/name_singular&gt;&lt;name_plural&gt;Industrial photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Tourismus</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A15])" office:value-type="string" office:string-value="tourismus" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tourismus</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A15]&amp;[Snippets.$C$17]&amp;[Translations.A15]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tourismus&lt;/name_singular&gt;&lt;name_plural&gt;Tourismus&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Tourismus&lt;/name_singular&gt;&lt;name_plural&gt;Tourismus&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B15]&amp;[Snippets.$C$18]&amp;[Translations.B15]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C15]&amp;[Snippets.$C$19]&amp;[Translations.C15]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D15]&amp;[Snippets.$C$20]&amp;[Translations.D15]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E15]&amp;[Snippets.$C$21]&amp;[Translations.E15]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B15]&amp;[Snippets.$C$18]&amp;[Translations.B15]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C15]&amp;[Snippets.$C$19]&amp;[Translations.C15]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D15]&amp;[Snippets.$C$20]&amp;[Translations.D15]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E15]&amp;[Snippets.$C$21]&amp;[Translations.E15]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B15]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;tourismus&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="tourismus" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H15]&amp;[Snippets.B$16]&amp;[.C15]&amp;[.D15]&amp;[.E15]&amp;[.F15]&amp;[.G15]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;tourismus&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tourismus&lt;/name_singular&gt;&lt;name_plural&gt;Tourismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="tourismus" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Tourismus&lt;/name_singular&gt;&lt;name_plural&gt;Tourismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H15]&amp;[Snippets.B$16]&amp;[.C15]&amp;[.D15]&amp;[.E15]&amp;[.F15]&amp;[.G15]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;tourismus&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tourismus&lt;/name_singular&gt;&lt;name_plural&gt;Tourismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="tourismus" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Tourismus&lt;/name_singular&gt;&lt;name_plural&gt;Tourismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Tourisme&lt;/name_singular&gt;&lt;name_plural&gt;Tourisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Turismo&lt;/name_singular&gt;&lt;name_plural&gt;Turismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Turissem&lt;/name_singular&gt;&lt;name_plural&gt;Turissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Tourism&lt;/name_singular&gt;&lt;name_plural&gt;Tourism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Landwirtschaft</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A16])" office:value-type="string" office:string-value="landwirtschaft" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>landwirtschaft</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A16]&amp;[Snippets.$C$17]&amp;[Translations.A16]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landwirtschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landwirtschaft&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Landwirtschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landwirtschaft&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B16]&amp;[Snippets.$C$18]&amp;[Translations.B16]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C16]&amp;[Snippets.$C$19]&amp;[Translations.C16]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D16]&amp;[Snippets.$C$20]&amp;[Translations.D16]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E16]&amp;[Snippets.$C$21]&amp;[Translations.E16]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B16]&amp;[Snippets.$C$18]&amp;[Translations.B16]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C16]&amp;[Snippets.$C$19]&amp;[Translations.C16]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D16]&amp;[Snippets.$C$20]&amp;[Translations.D16]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E16]&amp;[Snippets.$C$21]&amp;[Translations.E16]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B16]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;landwirtschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="landwirtschaft" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H16]&amp;[Snippets.B$16]&amp;[.C16]&amp;[.D16]&amp;[.E16]&amp;[.F16]&amp;[.G16]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;landwirtschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landwirtschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landwirtschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="landwirtschaft" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Landwirtschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landwirtschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H16]&amp;[Snippets.B$16]&amp;[.C16]&amp;[.D16]&amp;[.E16]&amp;[.F16]&amp;[.G16]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;landwirtschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Landwirtschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landwirtschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="landwirtschaft" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Landwirtschaft&lt;/name_singular&gt;&lt;name_plural&gt;Landwirtschaft&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Agricoltura&lt;/name_singular&gt;&lt;name_plural&gt;Agricoltura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Agricultura&lt;/name_singular&gt;&lt;name_plural&gt;Agricultura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Agriculture&lt;/name_singular&gt;&lt;name_plural&gt;Agriculture&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Tiere</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A17])" office:value-type="string" office:string-value="tiere" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>tiere</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A17]&amp;[Snippets.$C$17]&amp;[Translations.A17]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tiere&lt;/name_singular&gt;&lt;name_plural&gt;Tiere&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Tiere&lt;/name_singular&gt;&lt;name_plural&gt;Tiere&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B17]&amp;[Snippets.$C$18]&amp;[Translations.B17]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C17]&amp;[Snippets.$C$19]&amp;[Translations.C17]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D17]&amp;[Snippets.$C$20]&amp;[Translations.D17]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E17]&amp;[Snippets.$C$21]&amp;[Translations.E17]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B17]&amp;[Snippets.$C$18]&amp;[Translations.B17]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C17]&amp;[Snippets.$C$19]&amp;[Translations.C17]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D17]&amp;[Snippets.$C$20]&amp;[Translations.D17]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E17]&amp;[Snippets.$C$21]&amp;[Translations.E17]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B17]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;tiere&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="tiere" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H17]&amp;[Snippets.B$16]&amp;[.C17]&amp;[.D17]&amp;[.E17]&amp;[.F17]&amp;[.G17]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;tiere&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tiere&lt;/name_singular&gt;&lt;name_plural&gt;Tiere&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="tiere" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Tiere&lt;/name_singular&gt;&lt;name_plural&gt;Tiere&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H17]&amp;[Snippets.B$16]&amp;[.C17]&amp;[.D17]&amp;[.E17]&amp;[.F17]&amp;[.G17]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;tiere&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Tiere&lt;/name_singular&gt;&lt;name_plural&gt;Tiere&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="tiere" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Tiere&lt;/name_singular&gt;&lt;name_plural&gt;Tiere&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie animalière&lt;/name_singular&gt;&lt;name_plural&gt;Photographie animalière&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia animale&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia animale&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Animals&lt;/name_singular&gt;&lt;name_plural&gt;Animals&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Sachaufnahme</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A18])" office:value-type="string" office:string-value="sachaufnahme" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>sachaufnahme</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A18]&amp;[Snippets.$C$17]&amp;[Translations.A18]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sachaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Sachaufnahme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Sachaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Sachaufnahme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B18]&amp;[Snippets.$C$18]&amp;[Translations.B18]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C18]&amp;[Snippets.$C$19]&amp;[Translations.C18]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D18]&amp;[Snippets.$C$20]&amp;[Translations.D18]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E18]&amp;[Snippets.$C$21]&amp;[Translations.E18]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B18]&amp;[Snippets.$C$18]&amp;[Translations.B18]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C18]&amp;[Snippets.$C$19]&amp;[Translations.C18]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D18]&amp;[Snippets.$C$20]&amp;[Translations.D18]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E18]&amp;[Snippets.$C$21]&amp;[Translations.E18]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B18]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;sachaufnahme&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="sachaufnahme" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H18]&amp;[Snippets.B$16]&amp;[.C18]&amp;[.D18]&amp;[.E18]&amp;[.F18]&amp;[.G18]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;sachaufnahme&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sachaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Sachaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="sachaufnahme" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Sachaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Sachaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H18]&amp;[Snippets.B$16]&amp;[.C18]&amp;[.D18]&amp;[.E18]&amp;[.F18]&amp;[.G18]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;sachaufnahme&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sachaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Sachaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="sachaufnahme" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Sachaufnahme&lt;/name_singular&gt;&lt;name_plural&gt;Sachaufnahme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Objet&lt;/name_singular&gt;&lt;name_plural&gt;Objet&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Oggettistica&lt;/name_singular&gt;&lt;name_plural&gt;Oggettistica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Object&lt;/name_singular&gt;&lt;name_plural&gt;Object&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Object photography&lt;/name_singular&gt;&lt;name_plural&gt;Object photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Reproduktion</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A19])" office:value-type="string" office:string-value="reproduktion" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>reproduktion</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A19]&amp;[Snippets.$C$17]&amp;[Translations.A19]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproduktion&lt;/name_singular&gt;&lt;name_plural&gt;Reproduktion&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reproduktion&lt;/name_singular&gt;&lt;name_plural&gt;Reproduktion&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B19]&amp;[Snippets.$C$18]&amp;[Translations.B19]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C19]&amp;[Snippets.$C$19]&amp;[Translations.C19]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D19]&amp;[Snippets.$C$20]&amp;[Translations.D19]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E19]&amp;[Snippets.$C$21]&amp;[Translations.E19]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B19]&amp;[Snippets.$C$18]&amp;[Translations.B19]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C19]&amp;[Snippets.$C$19]&amp;[Translations.C19]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D19]&amp;[Snippets.$C$20]&amp;[Translations.D19]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E19]&amp;[Snippets.$C$21]&amp;[Translations.E19]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B19]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;reproduktion&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="reproduktion" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H19]&amp;[Snippets.B$16]&amp;[.C19]&amp;[.D19]&amp;[.E19]&amp;[.F19]&amp;[.G19]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;reproduktion&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproduktion&lt;/name_singular&gt;&lt;name_plural&gt;Reproduktion&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="reproduktion" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reproduktion&lt;/name_singular&gt;&lt;name_plural&gt;Reproduktion&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H19]&amp;[Snippets.B$16]&amp;[.C19]&amp;[.D19]&amp;[.E19]&amp;[.F19]&amp;[.G19]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;reproduktion&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproduktion&lt;/name_singular&gt;&lt;name_plural&gt;Reproduktion&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="reproduktion" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reproduktion&lt;/name_singular&gt;&lt;name_plural&gt;Reproduktion&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Riproduzione&lt;/name_singular&gt;&lt;name_plural&gt;Riproduzione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Reproducziun&lt;/name_singular&gt;&lt;name_plural&gt;Reproducziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Reproduction&lt;/name_singular&gt;&lt;name_plural&gt;Reproduction&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Werbung</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A20])" office:value-type="string" office:string-value="werbung" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>werbung</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A20]&amp;[Snippets.$C$17]&amp;[Translations.A20]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Werbung&lt;/name_singular&gt;&lt;name_plural&gt;Werbung&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Werbung&lt;/name_singular&gt;&lt;name_plural&gt;Werbung&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B20]&amp;[Snippets.$C$18]&amp;[Translations.B20]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C20]&amp;[Snippets.$C$19]&amp;[Translations.C20]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D20]&amp;[Snippets.$C$20]&amp;[Translations.D20]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E20]&amp;[Snippets.$C$21]&amp;[Translations.E20]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B20]&amp;[Snippets.$C$18]&amp;[Translations.B20]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C20]&amp;[Snippets.$C$19]&amp;[Translations.C20]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D20]&amp;[Snippets.$C$20]&amp;[Translations.D20]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E20]&amp;[Snippets.$C$21]&amp;[Translations.E20]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B20]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;werbung&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="werbung" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H20]&amp;[Snippets.B$16]&amp;[.C20]&amp;[.D20]&amp;[.E20]&amp;[.F20]&amp;[.G20]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;werbung&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Werbung&lt;/name_singular&gt;&lt;name_plural&gt;Werbung&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="werbung" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Werbung&lt;/name_singular&gt;&lt;name_plural&gt;Werbung&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H20]&amp;[Snippets.B$16]&amp;[.C20]&amp;[.D20]&amp;[.E20]&amp;[.F20]&amp;[.G20]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;werbung&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Werbung&lt;/name_singular&gt;&lt;name_plural&gt;Werbung&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="werbung" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Werbung&lt;/name_singular&gt;&lt;name_plural&gt;Werbung&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Publicité&lt;/name_singular&gt;&lt;name_plural&gt;Publicité&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Pubblicità&lt;/name_singular&gt;&lt;name_plural&gt;Pubblicità&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Reclama&lt;/name_singular&gt;&lt;name_plural&gt;Reclama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Publicity&lt;/name_singular&gt;&lt;name_plural&gt;Publicity&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Mode</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A21])" office:value-type="string" office:string-value="mode" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>mode</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A21]&amp;[Snippets.$C$17]&amp;[Translations.A21]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B21]&amp;[Snippets.$C$18]&amp;[Translations.B21]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C21]&amp;[Snippets.$C$19]&amp;[Translations.C21]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D21]&amp;[Snippets.$C$20]&amp;[Translations.D21]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E21]&amp;[Snippets.$C$21]&amp;[Translations.E21]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B21]&amp;[Snippets.$C$18]&amp;[Translations.B21]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C21]&amp;[Snippets.$C$19]&amp;[Translations.C21]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D21]&amp;[Snippets.$C$20]&amp;[Translations.D21]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E21]&amp;[Snippets.$C$21]&amp;[Translations.E21]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B21]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;mode&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="mode" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H21]&amp;[Snippets.B$16]&amp;[.C21]&amp;[.D21]&amp;[.E21]&amp;[.F21]&amp;[.G21]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;mode&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="mode" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H21]&amp;[Snippets.B$16]&amp;[.C21]&amp;[.D21]&amp;[.E21]&amp;[.F21]&amp;[.G21]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;mode&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="mode" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Mode&lt;/name_singular&gt;&lt;name_plural&gt;Mode&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Moda&lt;/name_singular&gt;&lt;name_plural&gt;Moda&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Fashion&lt;/name_singular&gt;&lt;name_plural&gt;Fashion&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
-            <text:p>Firmenportraet</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A22])" office:value-type="string" office:string-value="firmenportraet" calcext:value-type="string">
+            <text:p>Firmenporträt</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>firmenportraet</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A22]&amp;[Snippets.$C$17]&amp;[Translations.A22]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Firmenporträt&lt;/name_singular&gt;&lt;name_plural&gt;Firmenporträt&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Firmenporträt&lt;/name_singular&gt;&lt;name_plural&gt;Firmenporträt&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B22]&amp;[Snippets.$C$18]&amp;[Translations.B22]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C22]&amp;[Snippets.$C$19]&amp;[Translations.C22]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D22]&amp;[Snippets.$C$20]&amp;[Translations.D22]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E22]&amp;[Snippets.$C$21]&amp;[Translations.E22]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B22]&amp;[Snippets.$C$18]&amp;[Translations.B22]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C22]&amp;[Snippets.$C$19]&amp;[Translations.C22]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D22]&amp;[Snippets.$C$20]&amp;[Translations.D22]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E22]&amp;[Snippets.$C$21]&amp;[Translations.E22]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B22]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;firmenportraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="firmenportraet" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H22]&amp;[Snippets.B$16]&amp;[.C22]&amp;[.D22]&amp;[.E22]&amp;[.F22]&amp;[.G22]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;firmenportraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Firmenporträt&lt;/name_singular&gt;&lt;name_plural&gt;Firmenporträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="firmenportraet" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Firmenporträt&lt;/name_singular&gt;&lt;name_plural&gt;Firmenporträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H22]&amp;[Snippets.B$16]&amp;[.C22]&amp;[.D22]&amp;[.E22]&amp;[.F22]&amp;[.G22]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;firmenportraet&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Firmenporträt&lt;/name_singular&gt;&lt;name_plural&gt;Firmenporträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="firmenportraet" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Firmenporträt&lt;/name_singular&gt;&lt;name_plural&gt;Firmenporträt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Portrait d'entreprise&lt;/name_singular&gt;&lt;name_plural&gt;Portrait d'entreprise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Ritratto d’impresa&lt;/name_singular&gt;&lt;name_plural&gt;Ritratto d’impresa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Purtret da firma&lt;/name_singular&gt;&lt;name_plural&gt;Purtret da firma&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Enterprise representation&lt;/name_singular&gt;&lt;name_plural&gt;Enterprise representation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Sport</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A23])" office:value-type="string" office:string-value="sport" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>sport</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A23]&amp;[Snippets.$C$17]&amp;[Translations.A23]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B23]&amp;[Snippets.$C$18]&amp;[Translations.B23]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C23]&amp;[Snippets.$C$19]&amp;[Translations.C23]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D23]&amp;[Snippets.$C$20]&amp;[Translations.D23]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E23]&amp;[Snippets.$C$21]&amp;[Translations.E23]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B23]&amp;[Snippets.$C$18]&amp;[Translations.B23]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C23]&amp;[Snippets.$C$19]&amp;[Translations.C23]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D23]&amp;[Snippets.$C$20]&amp;[Translations.D23]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E23]&amp;[Snippets.$C$21]&amp;[Translations.E23]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B23]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;sport&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="sport" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H23]&amp;[Snippets.B$16]&amp;[.C23]&amp;[.D23]&amp;[.E23]&amp;[.F23]&amp;[.G23]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;sport&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="sport" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H23]&amp;[Snippets.B$16]&amp;[.C23]&amp;[.D23]&amp;[.E23]&amp;[.F23]&amp;[.G23]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;sport&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="sport" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Sport&lt;/name_singular&gt;&lt;name_plural&gt;Sport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Sports&lt;/name_singular&gt;&lt;name_plural&gt;Sports&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
-            <text:p>Unfall / Katastrophe</text:p>
+            <text:p>Unfall/Katastrophe</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>unfall</text:p>
@@ -713,342 +720,342 @@
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A24]&amp;[Snippets.$C$17]&amp;[Translations.A24]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Unfall/Katastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Unfall/Katastrophe&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Unfall/Katastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Unfall/Katastrophe&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B24]&amp;[Snippets.$C$18]&amp;[Translations.B24]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C24]&amp;[Snippets.$C$19]&amp;[Translations.C24]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D24]&amp;[Snippets.$C$20]&amp;[Translations.D24]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E24]&amp;[Snippets.$C$21]&amp;[Translations.E24]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B24]&amp;[Snippets.$C$18]&amp;[Translations.B24]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C24]&amp;[Snippets.$C$19]&amp;[Translations.C24]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D24]&amp;[Snippets.$C$20]&amp;[Translations.D24]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E24]&amp;[Snippets.$C$21]&amp;[Translations.E24]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B24]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;unfall&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="unfall" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H24]&amp;[Snippets.B$16]&amp;[.C24]&amp;[.D24]&amp;[.E24]&amp;[.F24]&amp;[.G24]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;unfall&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Unfall/Katastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Unfall/Katastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="unfall" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Unfall/Katastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Unfall/Katastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H24]&amp;[Snippets.B$16]&amp;[.C24]&amp;[.D24]&amp;[.E24]&amp;[.F24]&amp;[.G24]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;unfall&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Unfall/Katastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Unfall/Katastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="unfall" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Unfall/Katastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Unfall/Katastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Accident/catastrophe&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Incidente/catastrofe&lt;/name_singular&gt;&lt;name_plural&gt;Incidente/catastrofe&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Accident/catastrofa&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrofa&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Accident/catastrophy&lt;/name_singular&gt;&lt;name_plural&gt;Accident/catastrophy&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Verkehr</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A25])" office:value-type="string" office:string-value="verkehr" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>verkehr</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A25]&amp;[Snippets.$C$17]&amp;[Translations.A25]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Verkehr&lt;/name_singular&gt;&lt;name_plural&gt;Verkehr&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Verkehr&lt;/name_singular&gt;&lt;name_plural&gt;Verkehr&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B25]&amp;[Snippets.$C$18]&amp;[Translations.B25]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C25]&amp;[Snippets.$C$19]&amp;[Translations.C25]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D25]&amp;[Snippets.$C$20]&amp;[Translations.D25]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E25]&amp;[Snippets.$C$21]&amp;[Translations.E25]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B25]&amp;[Snippets.$C$18]&amp;[Translations.B25]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C25]&amp;[Snippets.$C$19]&amp;[Translations.C25]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D25]&amp;[Snippets.$C$20]&amp;[Translations.D25]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E25]&amp;[Snippets.$C$21]&amp;[Translations.E25]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B25]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;verkehr&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="verkehr" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H25]&amp;[Snippets.B$16]&amp;[.C25]&amp;[.D25]&amp;[.E25]&amp;[.F25]&amp;[.G25]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;verkehr&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Verkehr&lt;/name_singular&gt;&lt;name_plural&gt;Verkehr&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="verkehr" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Verkehr&lt;/name_singular&gt;&lt;name_plural&gt;Verkehr&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H25]&amp;[Snippets.B$16]&amp;[.C25]&amp;[.D25]&amp;[.E25]&amp;[.F25]&amp;[.G25]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;verkehr&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Verkehr&lt;/name_singular&gt;&lt;name_plural&gt;Verkehr&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="verkehr" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Verkehr&lt;/name_singular&gt;&lt;name_plural&gt;Verkehr&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Transport&lt;/name_singular&gt;&lt;name_plural&gt;Transport&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Trasporti&lt;/name_singular&gt;&lt;name_plural&gt;Trasporti&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Traffic&lt;/name_singular&gt;&lt;name_plural&gt;Traffic&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
-            <text:p>Militaer</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A26])" office:value-type="string" office:string-value="militaer" calcext:value-type="string">
+            <text:p>Militär</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>militaer</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A26]&amp;[Snippets.$C$17]&amp;[Translations.A26]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militär&lt;/name_singular&gt;&lt;name_plural&gt;Militär&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Militär&lt;/name_singular&gt;&lt;name_plural&gt;Militär&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B26]&amp;[Snippets.$C$18]&amp;[Translations.B26]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C26]&amp;[Snippets.$C$19]&amp;[Translations.C26]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D26]&amp;[Snippets.$C$20]&amp;[Translations.D26]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E26]&amp;[Snippets.$C$21]&amp;[Translations.E26]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B26]&amp;[Snippets.$C$18]&amp;[Translations.B26]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C26]&amp;[Snippets.$C$19]&amp;[Translations.C26]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D26]&amp;[Snippets.$C$20]&amp;[Translations.D26]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E26]&amp;[Snippets.$C$21]&amp;[Translations.E26]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B26]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;militaer&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="militaer" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H26]&amp;[Snippets.B$16]&amp;[.C26]&amp;[.D26]&amp;[.E26]&amp;[.F26]&amp;[.G26]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;militaer&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militär&lt;/name_singular&gt;&lt;name_plural&gt;Militär&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="militaer" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Militär&lt;/name_singular&gt;&lt;name_plural&gt;Militär&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H26]&amp;[Snippets.B$16]&amp;[.C26]&amp;[.D26]&amp;[.E26]&amp;[.F26]&amp;[.G26]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;militaer&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militär&lt;/name_singular&gt;&lt;name_plural&gt;Militär&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="militaer" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Militär&lt;/name_singular&gt;&lt;name_plural&gt;Militär&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Militaire&lt;/name_singular&gt;&lt;name_plural&gt;Militaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Militare&lt;/name_singular&gt;&lt;name_plural&gt;Militare&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Militar&lt;/name_singular&gt;&lt;name_plural&gt;Militar&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Military&lt;/name_singular&gt;&lt;name_plural&gt;Military&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Ethnologie</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A27])" office:value-type="string" office:string-value="ethnologie" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ethnologie</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A27]&amp;[Snippets.$C$17]&amp;[Translations.A27]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B27]&amp;[Snippets.$C$18]&amp;[Translations.B27]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C27]&amp;[Snippets.$C$19]&amp;[Translations.C27]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D27]&amp;[Snippets.$C$20]&amp;[Translations.D27]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E27]&amp;[Snippets.$C$21]&amp;[Translations.E27]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B27]&amp;[Snippets.$C$18]&amp;[Translations.B27]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C27]&amp;[Snippets.$C$19]&amp;[Translations.C27]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D27]&amp;[Snippets.$C$20]&amp;[Translations.D27]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E27]&amp;[Snippets.$C$21]&amp;[Translations.E27]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B27]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;ethnologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="ethnologie" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H27]&amp;[Snippets.B$16]&amp;[.C27]&amp;[.D27]&amp;[.E27]&amp;[.F27]&amp;[.G27]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;ethnologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="ethnologie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H27]&amp;[Snippets.B$16]&amp;[.C27]&amp;[.D27]&amp;[.E27]&amp;[.F27]&amp;[.G27]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;ethnologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="ethnologie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Ethnologie&lt;/name_singular&gt;&lt;name_plural&gt;Ethnologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Etnologia&lt;/name_singular&gt;&lt;name_plural&gt;Etnologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Anthropology&lt;/name_singular&gt;&lt;name_plural&gt;Anthropology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
-            <text:p>Archaeologie</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce1" table:formula="of:=LOWER([.A28])" office:value-type="string" office:string-value="archaeologie" calcext:value-type="string">
+            <text:p>Archäologie</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>archaeologie</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A28]&amp;[Snippets.$C$17]&amp;[Translations.A28]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archäologie&lt;/name_singular&gt;&lt;name_plural&gt;Archäologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Archäologie&lt;/name_singular&gt;&lt;name_plural&gt;Archäologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B28]&amp;[Snippets.$C$18]&amp;[Translations.B28]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C28]&amp;[Snippets.$C$19]&amp;[Translations.C28]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D28]&amp;[Snippets.$C$20]&amp;[Translations.D28]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E28]&amp;[Snippets.$C$21]&amp;[Translations.E28]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B28]&amp;[Snippets.$C$18]&amp;[Translations.B28]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C28]&amp;[Snippets.$C$19]&amp;[Translations.C28]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D28]&amp;[Snippets.$C$20]&amp;[Translations.D28]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E28]&amp;[Snippets.$C$21]&amp;[Translations.E28]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B28]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;archaeologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="archaeologie" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H28]&amp;[Snippets.B$16]&amp;[.C28]&amp;[.D28]&amp;[.E28]&amp;[.F28]&amp;[.G28]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;archaeologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archäologie&lt;/name_singular&gt;&lt;name_plural&gt;Archäologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="archaeologie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Archäologie&lt;/name_singular&gt;&lt;name_plural&gt;Archäologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H28]&amp;[Snippets.B$16]&amp;[.C28]&amp;[.D28]&amp;[.E28]&amp;[.F28]&amp;[.G28]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;archaeologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archäologie&lt;/name_singular&gt;&lt;name_plural&gt;Archäologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="archaeologie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Archäologie&lt;/name_singular&gt;&lt;name_plural&gt;Archäologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Archéologie&lt;/name_singular&gt;&lt;name_plural&gt;Archéologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Archeologia&lt;/name_singular&gt;&lt;name_plural&gt;Archeologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Archaeology&lt;/name_singular&gt;&lt;name_plural&gt;Archaeology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Medizin</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A29])" office:value-type="string" office:string-value="medizin" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>medizin</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A29]&amp;[Snippets.$C$17]&amp;[Translations.A29]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medizin&lt;/name_singular&gt;&lt;name_plural&gt;Medizin&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Medizin&lt;/name_singular&gt;&lt;name_plural&gt;Medizin&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B29]&amp;[Snippets.$C$18]&amp;[Translations.B29]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C29]&amp;[Snippets.$C$19]&amp;[Translations.C29]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D29]&amp;[Snippets.$C$20]&amp;[Translations.D29]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E29]&amp;[Snippets.$C$21]&amp;[Translations.E29]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B29]&amp;[Snippets.$C$18]&amp;[Translations.B29]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C29]&amp;[Snippets.$C$19]&amp;[Translations.C29]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D29]&amp;[Snippets.$C$20]&amp;[Translations.D29]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E29]&amp;[Snippets.$C$21]&amp;[Translations.E29]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B29]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;medizin&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="medizin" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H29]&amp;[Snippets.B$16]&amp;[.C29]&amp;[.D29]&amp;[.E29]&amp;[.F29]&amp;[.G29]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;medizin&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medizin&lt;/name_singular&gt;&lt;name_plural&gt;Medizin&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="medizin" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Medizin&lt;/name_singular&gt;&lt;name_plural&gt;Medizin&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H29]&amp;[Snippets.B$16]&amp;[.C29]&amp;[.D29]&amp;[.E29]&amp;[.F29]&amp;[.G29]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;medizin&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medizin&lt;/name_singular&gt;&lt;name_plural&gt;Medizin&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="medizin" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Medizin&lt;/name_singular&gt;&lt;name_plural&gt;Medizin&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Médecine&lt;/name_singular&gt;&lt;name_plural&gt;Médecine&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Medicina&lt;/name_singular&gt;&lt;name_plural&gt;Medicina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Medischina&lt;/name_singular&gt;&lt;name_plural&gt;Medischina&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Medicine&lt;/name_singular&gt;&lt;name_plural&gt;Medicine&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Kriminologie</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A30])" office:value-type="string" office:string-value="kriminologie" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>kriminologie</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A30]&amp;[Snippets.$C$17]&amp;[Translations.A30]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kriminologie&lt;/name_singular&gt;&lt;name_plural&gt;Kriminologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kriminologie&lt;/name_singular&gt;&lt;name_plural&gt;Kriminologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B30]&amp;[Snippets.$C$18]&amp;[Translations.B30]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C30]&amp;[Snippets.$C$19]&amp;[Translations.C30]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D30]&amp;[Snippets.$C$20]&amp;[Translations.D30]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E30]&amp;[Snippets.$C$21]&amp;[Translations.E30]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B30]&amp;[Snippets.$C$18]&amp;[Translations.B30]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C30]&amp;[Snippets.$C$19]&amp;[Translations.C30]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D30]&amp;[Snippets.$C$20]&amp;[Translations.D30]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E30]&amp;[Snippets.$C$21]&amp;[Translations.E30]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B30]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;kriminologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="kriminologie" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H30]&amp;[Snippets.B$16]&amp;[.C30]&amp;[.D30]&amp;[.E30]&amp;[.F30]&amp;[.G30]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;kriminologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kriminologie&lt;/name_singular&gt;&lt;name_plural&gt;Kriminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="kriminologie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kriminologie&lt;/name_singular&gt;&lt;name_plural&gt;Kriminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H30]&amp;[Snippets.B$16]&amp;[.C30]&amp;[.D30]&amp;[.E30]&amp;[.F30]&amp;[.G30]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;kriminologie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kriminologie&lt;/name_singular&gt;&lt;name_plural&gt;Kriminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="kriminologie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kriminologie&lt;/name_singular&gt;&lt;name_plural&gt;Kriminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Criminologie&lt;/name_singular&gt;&lt;name_plural&gt;Criminologie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Criminologia&lt;/name_singular&gt;&lt;name_plural&gt;Criminologia&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Criminology&lt;/name_singular&gt;&lt;name_plural&gt;Criminology&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Musik</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A31])" office:value-type="string" office:string-value="musik" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>musik</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A31]&amp;[Snippets.$C$17]&amp;[Translations.A31]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musik&lt;/name_singular&gt;&lt;name_plural&gt;Musik&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Musik&lt;/name_singular&gt;&lt;name_plural&gt;Musik&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B31]&amp;[Snippets.$C$18]&amp;[Translations.B31]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C31]&amp;[Snippets.$C$19]&amp;[Translations.C31]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D31]&amp;[Snippets.$C$20]&amp;[Translations.D31]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E31]&amp;[Snippets.$C$21]&amp;[Translations.E31]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B31]&amp;[Snippets.$C$18]&amp;[Translations.B31]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C31]&amp;[Snippets.$C$19]&amp;[Translations.C31]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D31]&amp;[Snippets.$C$20]&amp;[Translations.D31]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E31]&amp;[Snippets.$C$21]&amp;[Translations.E31]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B31]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;musik&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="musik" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H31]&amp;[Snippets.B$16]&amp;[.C31]&amp;[.D31]&amp;[.E31]&amp;[.F31]&amp;[.G31]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;musik&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musik&lt;/name_singular&gt;&lt;name_plural&gt;Musik&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="musik" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Musik&lt;/name_singular&gt;&lt;name_plural&gt;Musik&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H31]&amp;[Snippets.B$16]&amp;[.C31]&amp;[.D31]&amp;[.E31]&amp;[.F31]&amp;[.G31]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;musik&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musik&lt;/name_singular&gt;&lt;name_plural&gt;Musik&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="musik" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Musik&lt;/name_singular&gt;&lt;name_plural&gt;Musik&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Musique&lt;/name_singular&gt;&lt;name_plural&gt;Musique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Musica&lt;/name_singular&gt;&lt;name_plural&gt;Musica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Music&lt;/name_singular&gt;&lt;name_plural&gt;Music&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Theater</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A32])" office:value-type="string" office:string-value="theater" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>theater</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A32]&amp;[Snippets.$C$17]&amp;[Translations.A32]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Theater&lt;/name_singular&gt;&lt;name_plural&gt;Theater&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Theater&lt;/name_singular&gt;&lt;name_plural&gt;Theater&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B32]&amp;[Snippets.$C$18]&amp;[Translations.B32]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Thé&amp;acirc;tre&lt;/name_singular&gt;&lt;name_plural&gt;Thé&amp;acirc;tre&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Thé&amp;acirc;tre&lt;/name_singular&gt;&lt;name_plural&gt;Thé&amp;acirc;tre&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C32]&amp;[Snippets.$C$19]&amp;[Translations.C32]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D32]&amp;[Snippets.$C$20]&amp;[Translations.D32]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E32]&amp;[Snippets.$C$21]&amp;[Translations.E32]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B32]&amp;[Snippets.$C$18]&amp;[Translations.B32]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Théâtre&lt;/name_singular&gt;&lt;name_plural&gt;Théâtre&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Théâtre&lt;/name_singular&gt;&lt;name_plural&gt;Théâtre&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C32]&amp;[Snippets.$C$19]&amp;[Translations.C32]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D32]&amp;[Snippets.$C$20]&amp;[Translations.D32]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E32]&amp;[Snippets.$C$21]&amp;[Translations.E32]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B32]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;theater&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="theater" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H32]&amp;[Snippets.B$16]&amp;[.C32]&amp;[.D32]&amp;[.E32]&amp;[.F32]&amp;[.G32]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;theater&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Theater&lt;/name_singular&gt;&lt;name_plural&gt;Theater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Thé&amp;acirc;tre&lt;/name_singular&gt;&lt;name_plural&gt;Thé&amp;acirc;tre&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="theater" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Theater&lt;/name_singular&gt;&lt;name_plural&gt;Theater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Thé&amp;acirc;tre&lt;/name_singular&gt;&lt;name_plural&gt;Thé&amp;acirc;tre&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H32]&amp;[Snippets.B$16]&amp;[.C32]&amp;[.D32]&amp;[.E32]&amp;[.F32]&amp;[.G32]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;theater&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Theater&lt;/name_singular&gt;&lt;name_plural&gt;Theater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Théâtre&lt;/name_singular&gt;&lt;name_plural&gt;Théâtre&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="theater" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Theater&lt;/name_singular&gt;&lt;name_plural&gt;Theater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Théâtre&lt;/name_singular&gt;&lt;name_plural&gt;Théâtre&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Teatro&lt;/name_singular&gt;&lt;name_plural&gt;Teatro&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Teater&lt;/name_singular&gt;&lt;name_plural&gt;Teater&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Theatre&lt;/name_singular&gt;&lt;name_plural&gt;Theatre&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Kunst</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A33])" office:value-type="string" office:string-value="kunst" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>kunst</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A33]&amp;[Snippets.$C$17]&amp;[Translations.A33]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kunst&lt;/name_singular&gt;&lt;name_plural&gt;Kunst&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kunst&lt;/name_singular&gt;&lt;name_plural&gt;Kunst&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B33]&amp;[Snippets.$C$18]&amp;[Translations.B33]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C33]&amp;[Snippets.$C$19]&amp;[Translations.C33]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D33]&amp;[Snippets.$C$20]&amp;[Translations.D33]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E33]&amp;[Snippets.$C$21]&amp;[Translations.E33]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B33]&amp;[Snippets.$C$18]&amp;[Translations.B33]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C33]&amp;[Snippets.$C$19]&amp;[Translations.C33]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D33]&amp;[Snippets.$C$20]&amp;[Translations.D33]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E33]&amp;[Snippets.$C$21]&amp;[Translations.E33]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B33]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;kunst&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="kunst" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H33]&amp;[Snippets.B$16]&amp;[.C33]&amp;[.D33]&amp;[.E33]&amp;[.F33]&amp;[.G33]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;kunst&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kunst&lt;/name_singular&gt;&lt;name_plural&gt;Kunst&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="kunst" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kunst&lt;/name_singular&gt;&lt;name_plural&gt;Kunst&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H33]&amp;[Snippets.B$16]&amp;[.C33]&amp;[.D33]&amp;[.E33]&amp;[.F33]&amp;[.G33]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;kunst&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kunst&lt;/name_singular&gt;&lt;name_plural&gt;Kunst&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="kunst" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kunst&lt;/name_singular&gt;&lt;name_plural&gt;Kunst&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Arte&lt;/name_singular&gt;&lt;name_plural&gt;Arte&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Art&lt;/name_singular&gt;&lt;name_plural&gt;Art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Literatur</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A34])" office:value-type="string" office:string-value="literatur" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>literatur</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A34]&amp;[Snippets.$C$17]&amp;[Translations.A34]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Literatur&lt;/name_singular&gt;&lt;name_plural&gt;Literatur&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Literatur&lt;/name_singular&gt;&lt;name_plural&gt;Literatur&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B34]&amp;[Snippets.$C$18]&amp;[Translations.B34]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C34]&amp;[Snippets.$C$19]&amp;[Translations.C34]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D34]&amp;[Snippets.$C$20]&amp;[Translations.D34]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E34]&amp;[Snippets.$C$21]&amp;[Translations.E34]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B34]&amp;[Snippets.$C$18]&amp;[Translations.B34]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C34]&amp;[Snippets.$C$19]&amp;[Translations.C34]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D34]&amp;[Snippets.$C$20]&amp;[Translations.D34]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E34]&amp;[Snippets.$C$21]&amp;[Translations.E34]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B34]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;literatur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="literatur" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H34]&amp;[Snippets.B$16]&amp;[.C34]&amp;[.D34]&amp;[.E34]&amp;[.F34]&amp;[.G34]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;literatur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Literatur&lt;/name_singular&gt;&lt;name_plural&gt;Literatur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="literatur" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Literatur&lt;/name_singular&gt;&lt;name_plural&gt;Literatur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H34]&amp;[Snippets.B$16]&amp;[.C34]&amp;[.D34]&amp;[.E34]&amp;[.F34]&amp;[.G34]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;literatur&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Literatur&lt;/name_singular&gt;&lt;name_plural&gt;Literatur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="literatur" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Literatur&lt;/name_singular&gt;&lt;name_plural&gt;Literatur&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Littérature&lt;/name_singular&gt;&lt;name_plural&gt;Littérature&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Letteratura&lt;/name_singular&gt;&lt;name_plural&gt;Letteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Litteratura&lt;/name_singular&gt;&lt;name_plural&gt;Litteratura&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Literature&lt;/name_singular&gt;&lt;name_plural&gt;Literature&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Piktorialismus</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A35])" office:value-type="string" office:string-value="piktorialismus" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>piktorialismus</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A35]&amp;[Snippets.$C$17]&amp;[Translations.A35]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Piktorialismus&lt;/name_singular&gt;&lt;name_plural&gt;Piktorialismus&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Piktorialismus&lt;/name_singular&gt;&lt;name_plural&gt;Piktorialismus&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B35]&amp;[Snippets.$C$18]&amp;[Translations.B35]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C35]&amp;[Snippets.$C$19]&amp;[Translations.C35]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D35]&amp;[Snippets.$C$20]&amp;[Translations.D35]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E35]&amp;[Snippets.$C$21]&amp;[Translations.E35]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B35]&amp;[Snippets.$C$18]&amp;[Translations.B35]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C35]&amp;[Snippets.$C$19]&amp;[Translations.C35]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D35]&amp;[Snippets.$C$20]&amp;[Translations.D35]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E35]&amp;[Snippets.$C$21]&amp;[Translations.E35]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B35]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;piktorialismus&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="piktorialismus" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H35]&amp;[Snippets.B$16]&amp;[.C35]&amp;[.D35]&amp;[.E35]&amp;[.F35]&amp;[.G35]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;piktorialismus&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Piktorialismus&lt;/name_singular&gt;&lt;name_plural&gt;Piktorialismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="piktorialismus" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Piktorialismus&lt;/name_singular&gt;&lt;name_plural&gt;Piktorialismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H35]&amp;[Snippets.B$16]&amp;[.C35]&amp;[.D35]&amp;[.E35]&amp;[.F35]&amp;[.G35]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;piktorialismus&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Piktorialismus&lt;/name_singular&gt;&lt;name_plural&gt;Piktorialismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="piktorialismus" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Piktorialismus&lt;/name_singular&gt;&lt;name_plural&gt;Piktorialismus&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Pictorialisme&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialisme&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Pittorialismo&lt;/name_singular&gt;&lt;name_plural&gt;Pittorialismo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Picturialissem&lt;/name_singular&gt;&lt;name_plural&gt;Picturialissem&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Pictorialism&lt;/name_singular&gt;&lt;name_plural&gt;Pictorialism&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
@@ -1061,168 +1068,168 @@
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A36]&amp;[Snippets.$C$17]&amp;[Translations.A36]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kunst mit Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;Kunst mit Fotografie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kunst mit Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;Kunst mit Fotografie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B36]&amp;[Snippets.$C$18]&amp;[Translations.B36]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C36]&amp;[Snippets.$C$19]&amp;[Translations.C36]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D36]&amp;[Snippets.$C$20]&amp;[Translations.D36]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E36]&amp;[Snippets.$C$21]&amp;[Translations.E36]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B36]&amp;[Snippets.$C$18]&amp;[Translations.B36]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C36]&amp;[Snippets.$C$19]&amp;[Translations.C36]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D36]&amp;[Snippets.$C$20]&amp;[Translations.D36]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E36]&amp;[Snippets.$C$21]&amp;[Translations.E36]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B36]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;kunst_fotografie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="kunst_fotografie" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H36]&amp;[Snippets.B$16]&amp;[.C36]&amp;[.D36]&amp;[.E36]&amp;[.F36]&amp;[.G36]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;kunst_fotografie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kunst mit Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;Kunst mit Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="kunst_fotografie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kunst mit Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;Kunst mit Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H36]&amp;[Snippets.B$16]&amp;[.C36]&amp;[.D36]&amp;[.E36]&amp;[.F36]&amp;[.G36]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;kunst_fotografie&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Kunst mit Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;Kunst mit Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="kunst_fotografie" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Kunst mit Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;Kunst mit Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Art photographique&lt;/name_singular&gt;&lt;name_plural&gt;Art photographique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Arte fotografica&lt;/name_singular&gt;&lt;name_plural&gt;Arte fotografica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Art fotografic&lt;/name_singular&gt;&lt;name_plural&gt;Art fotografic&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Photographic art&lt;/name_singular&gt;&lt;name_plural&gt;Photographic art&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Alltag</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A37])" office:value-type="string" office:string-value="alltag" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>alltag</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A37]&amp;[Snippets.$C$17]&amp;[Translations.A37]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Alltag&lt;/name_singular&gt;&lt;name_plural&gt;Alltag&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Alltag&lt;/name_singular&gt;&lt;name_plural&gt;Alltag&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B37]&amp;[Snippets.$C$18]&amp;[Translations.B37]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C37]&amp;[Snippets.$C$19]&amp;[Translations.C37]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D37]&amp;[Snippets.$C$20]&amp;[Translations.D37]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E37]&amp;[Snippets.$C$21]&amp;[Translations.E37]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B37]&amp;[Snippets.$C$18]&amp;[Translations.B37]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C37]&amp;[Snippets.$C$19]&amp;[Translations.C37]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D37]&amp;[Snippets.$C$20]&amp;[Translations.D37]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E37]&amp;[Snippets.$C$21]&amp;[Translations.E37]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B37]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;alltag&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="alltag" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H37]&amp;[Snippets.B$16]&amp;[.C37]&amp;[.D37]&amp;[.E37]&amp;[.F37]&amp;[.G37]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;alltag&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Alltag&lt;/name_singular&gt;&lt;name_plural&gt;Alltag&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="alltag" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Alltag&lt;/name_singular&gt;&lt;name_plural&gt;Alltag&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H37]&amp;[Snippets.B$16]&amp;[.C37]&amp;[.D37]&amp;[.E37]&amp;[.F37]&amp;[.G37]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;alltag&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Alltag&lt;/name_singular&gt;&lt;name_plural&gt;Alltag&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="alltag" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Alltag&lt;/name_singular&gt;&lt;name_plural&gt;Alltag&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Vie quotidienne&lt;/name_singular&gt;&lt;name_plural&gt;Vie quotidienne&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Vita quotidiana&lt;/name_singular&gt;&lt;name_plural&gt;Vita quotidiana&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Mintgadi&lt;/name_singular&gt;&lt;name_plural&gt;Mintgadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Everyday life&lt;/name_singular&gt;&lt;name_plural&gt;Everyday life&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Akt</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A38])" office:value-type="string" office:string-value="akt" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>akt</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A38]&amp;[Snippets.$C$17]&amp;[Translations.A38]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Akt&lt;/name_singular&gt;&lt;name_plural&gt;Akt&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Akt&lt;/name_singular&gt;&lt;name_plural&gt;Akt&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B38]&amp;[Snippets.$C$18]&amp;[Translations.B38]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C38]&amp;[Snippets.$C$19]&amp;[Translations.C38]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D38]&amp;[Snippets.$C$20]&amp;[Translations.D38]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E38]&amp;[Snippets.$C$21]&amp;[Translations.E38]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B38]&amp;[Snippets.$C$18]&amp;[Translations.B38]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C38]&amp;[Snippets.$C$19]&amp;[Translations.C38]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D38]&amp;[Snippets.$C$20]&amp;[Translations.D38]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E38]&amp;[Snippets.$C$21]&amp;[Translations.E38]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B38]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;akt&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="akt" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H38]&amp;[Snippets.B$16]&amp;[.C38]&amp;[.D38]&amp;[.E38]&amp;[.F38]&amp;[.G38]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;akt&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Akt&lt;/name_singular&gt;&lt;name_plural&gt;Akt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="akt" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Akt&lt;/name_singular&gt;&lt;name_plural&gt;Akt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H38]&amp;[Snippets.B$16]&amp;[.C38]&amp;[.D38]&amp;[.E38]&amp;[.F38]&amp;[.G38]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;akt&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Akt&lt;/name_singular&gt;&lt;name_plural&gt;Akt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="akt" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Akt&lt;/name_singular&gt;&lt;name_plural&gt;Akt&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Nu&lt;/name_singular&gt;&lt;name_plural&gt;Nu&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Nudo&lt;/name_singular&gt;&lt;name_plural&gt;Nudo&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Niv&lt;/name_singular&gt;&lt;name_plural&gt;Niv&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Act&lt;/name_singular&gt;&lt;name_plural&gt;Act&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Film</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A39])" office:value-type="string" office:string-value="film" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>film</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A39]&amp;[Snippets.$C$17]&amp;[Translations.A39]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B39]&amp;[Snippets.$C$18]&amp;[Translations.B39]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C39]&amp;[Snippets.$C$19]&amp;[Translations.C39]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D39]&amp;[Snippets.$C$20]&amp;[Translations.D39]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E39]&amp;[Snippets.$C$21]&amp;[Translations.E39]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B39]&amp;[Snippets.$C$18]&amp;[Translations.B39]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C39]&amp;[Snippets.$C$19]&amp;[Translations.C39]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D39]&amp;[Snippets.$C$20]&amp;[Translations.D39]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E39]&amp;[Snippets.$C$21]&amp;[Translations.E39]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B39]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;film&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="film" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H39]&amp;[Snippets.B$16]&amp;[.C39]&amp;[.D39]&amp;[.E39]&amp;[.F39]&amp;[.G39]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;film&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="film" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H39]&amp;[Snippets.B$16]&amp;[.C39]&amp;[.D39]&amp;[.E39]&amp;[.F39]&amp;[.G39]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;film&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="film" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Film&lt;/name_singular&gt;&lt;name_plural&gt;Film&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Movie&lt;/name_singular&gt;&lt;name_plural&gt;Movie&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Dokumentation</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A40])" office:value-type="string" office:string-value="dokumentation" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>dokumentation</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A40]&amp;[Snippets.$C$17]&amp;[Translations.A40]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Dokumentation&lt;/name_singular&gt;&lt;name_plural&gt;Dokumentation&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Dokumentation&lt;/name_singular&gt;&lt;name_plural&gt;Dokumentation&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B40]&amp;[Snippets.$C$18]&amp;[Translations.B40]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C40]&amp;[Snippets.$C$19]&amp;[Translations.C40]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D40]&amp;[Snippets.$C$20]&amp;[Translations.D40]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E40]&amp;[Snippets.$C$21]&amp;[Translations.E40]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B40]&amp;[Snippets.$C$18]&amp;[Translations.B40]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C40]&amp;[Snippets.$C$19]&amp;[Translations.C40]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D40]&amp;[Snippets.$C$20]&amp;[Translations.D40]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E40]&amp;[Snippets.$C$21]&amp;[Translations.E40]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B40]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;dokumentation&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="dokumentation" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H40]&amp;[Snippets.B$16]&amp;[.C40]&amp;[.D40]&amp;[.E40]&amp;[.F40]&amp;[.G40]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;dokumentation&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Dokumentation&lt;/name_singular&gt;&lt;name_plural&gt;Dokumentation&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="dokumentation" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Dokumentation&lt;/name_singular&gt;&lt;name_plural&gt;Dokumentation&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H40]&amp;[Snippets.B$16]&amp;[.C40]&amp;[.D40]&amp;[.E40]&amp;[.F40]&amp;[.G40]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;dokumentation&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Dokumentation&lt;/name_singular&gt;&lt;name_plural&gt;Dokumentation&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="dokumentation" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Dokumentation&lt;/name_singular&gt;&lt;name_plural&gt;Dokumentation&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie documentaire&lt;/name_singular&gt;&lt;name_plural&gt;Photographie documentaire&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia documentaria&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia documentaria&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Documentaziun&lt;/name_singular&gt;&lt;name_plural&gt;Documentaziun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Documentation&lt;/name_singular&gt;&lt;name_plural&gt;Documentation&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Multivision</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A41])" office:value-type="string" office:string-value="multivision" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>multivision</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A41]&amp;[Snippets.$C$17]&amp;[Translations.A41]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B41]&amp;[Snippets.$C$18]&amp;[Translations.B41]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C41]&amp;[Snippets.$C$19]&amp;[Translations.C41]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D41]&amp;[Snippets.$C$20]&amp;[Translations.D41]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E41]&amp;[Snippets.$C$21]&amp;[Translations.E41]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B41]&amp;[Snippets.$C$18]&amp;[Translations.B41]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C41]&amp;[Snippets.$C$19]&amp;[Translations.C41]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D41]&amp;[Snippets.$C$20]&amp;[Translations.D41]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E41]&amp;[Snippets.$C$21]&amp;[Translations.E41]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B41]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;multivision&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="multivision" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H41]&amp;[Snippets.B$16]&amp;[.C41]&amp;[.D41]&amp;[.E41]&amp;[.F41]&amp;[.G41]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;multivision&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="multivision" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H41]&amp;[Snippets.B$16]&amp;[.C41]&amp;[.D41]&amp;[.E41]&amp;[.F41]&amp;[.G41]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;multivision&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="multivision" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Diaporama&lt;/name_singular&gt;&lt;name_plural&gt;Diaporama&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Multivisione&lt;/name_singular&gt;&lt;name_plural&gt;Multivisione&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Multivisiun&lt;/name_singular&gt;&lt;name_plural&gt;Multivisiun&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Multivision&lt;/name_singular&gt;&lt;name_plural&gt;Multivision&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
@@ -1235,23 +1242,23 @@
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A42]&amp;[Snippets.$C$17]&amp;[Translations.A42]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;private Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;private Fotografie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;private Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;private Fotografie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B42]&amp;[Snippets.$C$18]&amp;[Translations.B42]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C42]&amp;[Snippets.$C$19]&amp;[Translations.C42]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D42]&amp;[Snippets.$C$20]&amp;[Translations.D42]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E42]&amp;[Snippets.$C$21]&amp;[Translations.E42]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B42]&amp;[Snippets.$C$18]&amp;[Translations.B42]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C42]&amp;[Snippets.$C$19]&amp;[Translations.C42]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D42]&amp;[Snippets.$C$20]&amp;[Translations.D42]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E42]&amp;[Snippets.$C$21]&amp;[Translations.E42]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B42]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;private&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="private" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H42]&amp;[Snippets.B$16]&amp;[.C42]&amp;[.D42]&amp;[.E42]&amp;[.F42]&amp;[.G42]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;private&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;private Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;private Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="private" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;private Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;private Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H42]&amp;[Snippets.B$16]&amp;[.C42]&amp;[.D42]&amp;[.E42]&amp;[.F42]&amp;[.G42]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;private&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;private Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;private Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="private" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;private Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;private Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie privée&lt;/name_singular&gt;&lt;name_plural&gt;Photographie privée&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia privata&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia privata&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Private photography&lt;/name_singular&gt;&lt;name_plural&gt;Private photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
@@ -1264,52 +1271,52 @@
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A43]&amp;[Snippets.$C$17]&amp;[Translations.A43]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;wissenschaftliche Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;wissenschaftliche Fotografie&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;wissenschaftliche Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;wissenschaftliche Fotografie&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B43]&amp;[Snippets.$C$18]&amp;[Translations.B43]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C43]&amp;[Snippets.$C$19]&amp;[Translations.C43]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D43]&amp;[Snippets.$C$20]&amp;[Translations.D43]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E43]&amp;[Snippets.$C$21]&amp;[Translations.E43]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B43]&amp;[Snippets.$C$18]&amp;[Translations.B43]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C43]&amp;[Snippets.$C$19]&amp;[Translations.C43]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D43]&amp;[Snippets.$C$20]&amp;[Translations.D43]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E43]&amp;[Snippets.$C$21]&amp;[Translations.E43]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B43]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;wissenschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="wissenschaft" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H43]&amp;[Snippets.B$16]&amp;[.C43]&amp;[.D43]&amp;[.E43]&amp;[.F43]&amp;[.G43]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;wissenschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;wissenschaftliche Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;wissenschaftliche Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="wissenschaft" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;wissenschaftliche Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;wissenschaftliche Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H43]&amp;[Snippets.B$16]&amp;[.C43]&amp;[.D43]&amp;[.E43]&amp;[.F43]&amp;[.G43]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;wissenschaft&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;wissenschaftliche Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;wissenschaftliche Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="wissenschaft" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;wissenschaftliche Fotografie&lt;/name_singular&gt;&lt;name_plural&gt;wissenschaftliche Fotografie&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Photographie scientifique&lt;/name_singular&gt;&lt;name_plural&gt;Photographie scientifique&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Fotografia scientifica&lt;/name_singular&gt;&lt;name_plural&gt;Fotografia scientifica&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Scientific photography&lt;/name_singular&gt;&lt;name_plural&gt;Scientific photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Reise</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=LOWER([.A44])" office:value-type="string" office:string-value="reise" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>reise</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.$B$17]&amp;[Translations.A44]&amp;[Snippets.$C$17]&amp;[Translations.A44]&amp;[Snippets.$D$17]" office:value-type="string" office:string-value="&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reise&lt;/name_singular&gt;&lt;name_plural&gt;Reise&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
             <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reise&lt;/name_singular&gt;&lt;name_plural&gt;Reise&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B44]&amp;[Snippets.$C$18]&amp;[Translations.B44]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C44]&amp;[Snippets.$C$19]&amp;[Translations.C44]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D44]&amp;[Snippets.$C$20]&amp;[Translations.D44]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E44]&amp;[Snippets.$C$21]&amp;[Translations.E44]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          <table:table-cell table:formula="of:=[Snippets.$B$18]&amp;[Translations.B44]&amp;[Snippets.$C$18]&amp;[Translations.B44]&amp;[Snippets.$D$18]" office:value-type="string" office:string-value="&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$19]&amp;[Translations.C44]&amp;[Snippets.$C$19]&amp;[Translations.C44]&amp;[Snippets.$D$19]" office:value-type="string" office:string-value="&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$20]&amp;[Translations.D44]&amp;[Snippets.$C$20]&amp;[Translations.D44]&amp;[Snippets.$D$20]" office:value-type="string" office:string-value="&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:formula="of:=[Snippets.$B$21]&amp;[Translations.E44]&amp;[Snippets.$C$21]&amp;[Translations.E44]&amp;[Snippets.$D$21]" office:value-type="string" office:string-value="&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;</text:p>
           </table:table-cell>
           <table:table-cell table:formula="of:=[Snippets.B$15]&amp;[.B44]&amp;[Snippets.C$15]" office:value-type="string" office:string-value="&lt;item idno=&quot;reise&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;" calcext:value-type="string">
             <text:p>&lt;item idno="reise" enabled="1" default="0" value="0"&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:formula="of:=[.H44]&amp;[Snippets.B$16]&amp;[.C44]&amp;[.D44]&amp;[.E44]&amp;[.F44]&amp;[.G44]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;reise&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reise&lt;/name_singular&gt;&lt;name_plural&gt;Reise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;0&quot;&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
-            <text:p>&lt;item idno="reise" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reise&lt;/name_singular&gt;&lt;name_plural&gt;Reise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
+          <table:table-cell table:formula="of:=[.H44]&amp;[Snippets.B$16]&amp;[.C44]&amp;[.D44]&amp;[.E44]&amp;[.F44]&amp;[.G44]&amp;[Snippets.B$22]&amp;[Snippets.B$23]" office:value-type="string" office:string-value="&lt;item idno=&quot;reise&quot; enabled=&quot;1&quot; default=&quot;0&quot; value=&quot;0&quot;&gt;&lt;labels&gt;&lt;label locale=&quot;de_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Reise&lt;/name_singular&gt;&lt;name_plural&gt;Reise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;fr_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;it_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;rm_CH&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale=&quot;en_US&quot; preferred=&quot;1&quot;&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;" calcext:value-type="string">
+            <text:p>&lt;item idno="reise" enabled="1" default="0" value="0"&gt;&lt;labels&gt;&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Reise&lt;/name_singular&gt;&lt;name_plural&gt;Reise&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;Voyage&lt;/name_singular&gt;&lt;name_plural&gt;Voyage&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;Viaggio&lt;/name_singular&gt;&lt;name_plural&gt;Viaggio&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;Viadi&lt;/name_singular&gt;&lt;name_plural&gt;Viadi&lt;/name_plural&gt;&lt;/label&gt;&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;Travelling photography&lt;/name_singular&gt;&lt;name_plural&gt;Travelling photography&lt;/name_plural&gt;&lt;/label&gt;&lt;/labels&gt;&lt;/item&gt;</text:p>
           </table:table-cell>
         </table:table-row>
       </table:table>
@@ -1785,7 +1792,7 @@
             <text:p>Theater</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Thé&amp;acirc;tre</text:p>
+            <text:p>Théâtre</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Teatro</text:p>
@@ -1985,203 +1992,183 @@
         </table:table-row>
       </table:table>
       <table:table table:name="Snippets" table:style-name="ta1">
-        <table:table-column table:style-name="co3" table:number-columns-repeated="6" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co3" table:number-columns-repeated="5" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>Example</text:p>
           </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;item idno="personen" enabled="1" default="0" value="0"&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;labels&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/labels&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/item&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3" table:number-rows-repeated="3">
           <table:table-cell table:number-columns-repeated="5"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;item idno="personen" enabled="1" default="0" value="0"&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>Snippets</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>B</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>C</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>D</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;item idno="</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>" enabled="1" default="0" value="0"&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
             <text:p>&lt;labels&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;Personen&lt;/name_singular&gt;&lt;name_plural&gt;Personen&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce8" table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="fr_CH" preferred="1"&gt;&lt;name_singular&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="it_CH" preferred="1"&gt;&lt;name_singular&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="rm_CH" preferred="1"&gt;&lt;name_singular&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;label locale="en_US" preferred="1"&gt;&lt;name_singular&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
+            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
             <text:p>&lt;/labels&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce8" table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8"/>
+          <table:table-cell table:style-name="ce8" office:value-type="string" calcext:value-type="string">
             <text:p>&lt;/item&gt;</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3" table:number-rows-repeated="3">
-          <table:table-cell table:number-columns-repeated="6"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
-            <text:p>Snippets</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>C</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>D</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>E</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>F</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B15</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;item idno="</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>" enabled="1" default="0" value="0"&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B16</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;labels&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="4"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B17</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="de_CH" preferred="1"&gt;&lt;name_singular&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B18</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="fr_CH" preferred="0"&gt;&lt;name_singular&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B19</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="it_CH" preferred="0"&gt;&lt;name_singular&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B20</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="rm_CH" preferred="0"&gt;&lt;name_singular&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B21</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;label locale="en_US" preferred="0"&gt;&lt;name_singular&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_singular&gt;&lt;name_plural&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/name_plural&gt;&lt;/label&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B22</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/labels&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="4"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro3">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>B23</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>&lt;/item&gt;</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell table:style-name="ce8" table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell table:style-name="ce8" table:number-columns-repeated="5"/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -2194,11 +2181,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2018-09-27T13:59:53.251000000</meta:creation-date>
-    <dc:date>2018-10-01T16:36:40.013000000</dc:date>
-    <meta:editing-duration>PT52M8S</meta:editing-duration>
-    <meta:editing-cycles>14</meta:editing-cycles>
+    <dc:date>2018-10-02T09:51:34.190000000</dc:date>
+    <meta:editing-duration>PT1H1M3S</meta:editing-duration>
+    <meta:editing-cycles>21</meta:editing-cycles>
     <meta:generator>LibreOffice/5.3.3.2$Windows_X86_64 LibreOffice_project/3d9a8b4b4e538a85e0782bd6c2d430bafe583448</meta:generator>
-    <meta:document-statistic meta:table-count="3" meta:cell-count="647" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="3" meta:cell-count="636" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -2217,7 +2204,7 @@
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Concat">
               <config:config-item config:name="CursorPositionX" config:type="int">8</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">26</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -2226,7 +2213,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">15</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -2234,8 +2221,8 @@
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="Snippets">
-              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">16</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">8</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -2253,7 +2240,7 @@
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="Translations">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">41</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -2455,9 +2442,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2018-10-01">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2018-10-02">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="16:11:13.401000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="09:42:37.384000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>